<commit_message>
Added another sheet that calculates dividers for given frequencies.  Upon experimentation, we will test the maximum distance those given dividers at given frequency offset provides.
</commit_message>
<xml_diff>
--- a/stats/fieldtestingparameters.xlsx
+++ b/stats/fieldtestingparameters.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fadde/Projects/wcnes-project2023/stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6823EADC-7E5B-6343-9BA1-6364525B61C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D506B176-5FAF-6A44-A092-397344376D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21360" yWindow="-28100" windowWidth="25300" windowHeight="27900" xr2:uid="{0E90CDDC-DED9-2445-AC68-A5DC0636EE53}"/>
+    <workbookView xWindow="25700" yWindow="14760" windowWidth="25300" windowHeight="13840" activeTab="1" xr2:uid="{0E90CDDC-DED9-2445-AC68-A5DC0636EE53}"/>
   </bookViews>
   <sheets>
     <sheet name="clicktoclick" sheetId="1" r:id="rId1"/>
+    <sheet name="Click&amp;Firefly" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,17 +24,42 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>f0 divider</t>
   </si>
@@ -66,13 +92,61 @@
   </si>
   <si>
     <t>default configuration</t>
+  </si>
+  <si>
+    <t>Baudrate R_b (kbps)</t>
+  </si>
+  <si>
+    <t>Carrier f_c (kHz)</t>
+  </si>
+  <si>
+    <t>Bandpass filter B_R (kHz)</t>
+  </si>
+  <si>
+    <t>Divider</t>
+  </si>
+  <si>
+    <t>Changing</t>
+  </si>
+  <si>
+    <t>Fixed Parameters:</t>
+  </si>
+  <si>
+    <t>freq deviation delta_FSK (kHz)</t>
+  </si>
+  <si>
+    <t>Results/notes from experiment</t>
+  </si>
+  <si>
+    <t>∆F_1</t>
+  </si>
+  <si>
+    <t>∆F_0</t>
+  </si>
+  <si>
+    <t>Receiver freq f_R (kHz)</t>
+  </si>
+  <si>
+    <t>∆f (kHz)</t>
+  </si>
+  <si>
+    <t>freq (MHz)</t>
+  </si>
+  <si>
+    <t>clock (MHz)</t>
+  </si>
+  <si>
+    <t>Center freq f_R (MHz)</t>
+  </si>
+  <si>
+    <t>Max D_1 (m)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -102,8 +176,72 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -116,8 +254,33 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -164,11 +327,113 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -184,11 +449,65 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="9" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
+    <cellStyle name="Accent1" xfId="5" builtinId="29"/>
+    <cellStyle name="Input" xfId="2" builtinId="20"/>
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="4" builtinId="10"/>
+    <cellStyle name="Output" xfId="3" builtinId="21"/>
   </cellStyles>
   <dxfs count="13">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -338,20 +657,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -393,7 +698,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5901A61B-C174-194B-9AE9-016534A343C6}" name="Table1" displayName="Table1" ref="A1:J15" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" headerRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5901A61B-C174-194B-9AE9-016534A343C6}" name="Table1" displayName="Table1" ref="A1:J15" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11">
   <autoFilter ref="A1:J15" xr:uid="{5901A61B-C174-194B-9AE9-016534A343C6}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{B10F3753-68C6-4648-BF58-A924DA03C465}" name="clock freq (Mhz)" dataDxfId="9"/>
@@ -720,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A2521C1-6B4D-B145-A199-3CB8A161D86E}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView zoomScale="75" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
@@ -1060,4 +1365,282 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{411A848C-79E9-A549-AF4C-929074E1F683}">
+  <dimension ref="A1:L9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="26" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="16"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="12"/>
+    </row>
+    <row r="2" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="11">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="22" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="13"/>
+      <c r="K3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="11">
+        <v>347.22222219999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <f>L6 + C4</f>
+        <v>2451000</v>
+      </c>
+      <c r="B4" cm="1">
+        <f t="array" ref="B4:B9">(H4:H9+E4:E9 )/2</f>
+        <v>0.99041445035460995</v>
+      </c>
+      <c r="C4">
+        <v>1000</v>
+      </c>
+      <c r="E4" cm="1">
+        <f t="array" ref="E4:E9">L2/F4:F9</f>
+        <v>0.65104166666666663</v>
+      </c>
+      <c r="F4" cm="1">
+        <f t="array" ref="F4:F9">EVEN((1000 * L2)/(C4:C9 - L3))</f>
+        <v>192</v>
+      </c>
+      <c r="H4" cm="1">
+        <f t="array" ref="H4:H9" xml:space="preserve"> L2/I4:I9</f>
+        <v>1.3297872340425532</v>
+      </c>
+      <c r="I4" cm="1">
+        <f t="array" ref="I4:I9">EVEN((1000 * L2)/(C4:C9 + L3))</f>
+        <v>94</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="11">
+        <f>2 *L3 + L5</f>
+        <v>794.44444439999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f>L6 + C5</f>
+        <v>2452000</v>
+      </c>
+      <c r="B5">
+        <v>1.9797758284600389</v>
+      </c>
+      <c r="C5">
+        <v>2000</v>
+      </c>
+      <c r="E5">
+        <v>1.6447368421052631</v>
+      </c>
+      <c r="F5">
+        <v>76</v>
+      </c>
+      <c r="H5">
+        <v>2.3148148148148149</v>
+      </c>
+      <c r="I5">
+        <v>54</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <f xml:space="preserve"> L6 + C6</f>
+        <v>2453000</v>
+      </c>
+      <c r="B6">
+        <v>2.9468201754385963</v>
+      </c>
+      <c r="C6">
+        <v>3000</v>
+      </c>
+      <c r="E6">
+        <v>2.6041666666666665</v>
+      </c>
+      <c r="F6">
+        <v>48</v>
+      </c>
+      <c r="H6">
+        <v>3.2894736842105261</v>
+      </c>
+      <c r="I6">
+        <v>38</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" s="11">
+        <v>2450000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <f>L6 + C7</f>
+        <v>2454000</v>
+      </c>
+      <c r="B7">
+        <v>3.8194444444444446</v>
+      </c>
+      <c r="C7">
+        <v>4000</v>
+      </c>
+      <c r="E7">
+        <v>3.4722222222222223</v>
+      </c>
+      <c r="F7">
+        <v>36</v>
+      </c>
+      <c r="H7">
+        <v>4.166666666666667</v>
+      </c>
+      <c r="I7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <f xml:space="preserve"> L6 + C8</f>
+        <v>2455000</v>
+      </c>
+      <c r="B8">
+        <v>4.8363095238095237</v>
+      </c>
+      <c r="C8">
+        <v>5000</v>
+      </c>
+      <c r="E8">
+        <v>4.4642857142857144</v>
+      </c>
+      <c r="F8">
+        <v>28</v>
+      </c>
+      <c r="H8">
+        <v>5.208333333333333</v>
+      </c>
+      <c r="I8">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <f>L6 + C9</f>
+        <v>2456000</v>
+      </c>
+      <c r="B9">
+        <v>5.7291666666666661</v>
+      </c>
+      <c r="C9">
+        <v>6000</v>
+      </c>
+      <c r="E9">
+        <v>5.208333333333333</v>
+      </c>
+      <c r="F9">
+        <v>24</v>
+      </c>
+      <c r="H9">
+        <v>6.25</v>
+      </c>
+      <c r="I9">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:J3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
did some measurements for click & firefly
</commit_message>
<xml_diff>
--- a/stats/fieldtestingparameters.xlsx
+++ b/stats/fieldtestingparameters.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fadde/Projects/wcnes-project2023/stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D506B176-5FAF-6A44-A092-397344376D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D887A5-16FB-F549-969C-C3D53270AD33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25700" yWindow="14760" windowWidth="25300" windowHeight="13840" activeTab="1" xr2:uid="{0E90CDDC-DED9-2445-AC68-A5DC0636EE53}"/>
+    <workbookView xWindow="1740" yWindow="1840" windowWidth="31100" windowHeight="19420" activeTab="2" xr2:uid="{0E90CDDC-DED9-2445-AC68-A5DC0636EE53}"/>
   </bookViews>
   <sheets>
     <sheet name="clicktoclick" sheetId="1" r:id="rId1"/>
-    <sheet name="Click&amp;Firefly" sheetId="2" r:id="rId2"/>
+    <sheet name="firefly&amp;launchpad" sheetId="2" r:id="rId2"/>
+    <sheet name="click&amp;firefly" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>f0 divider</t>
   </si>
@@ -140,13 +141,43 @@
   </si>
   <si>
     <t>Max D_1 (m)</t>
+  </si>
+  <si>
+    <t>Max D_0 (m)</t>
+  </si>
+  <si>
+    <t>bit reliability (%)</t>
+  </si>
+  <si>
+    <t>50k</t>
+  </si>
+  <si>
+    <t>75k</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>125k</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>Baudrate</t>
+  </si>
+  <si>
+    <t>bit reliability (%) @ 0.6m @ 24 22</t>
+  </si>
+  <si>
+    <t>bit reliability (%) @ 0.6m @ 30 28</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -240,8 +271,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,6 +316,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
       </patternFill>
     </fill>
   </fills>
@@ -425,15 +469,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -449,22 +494,25 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="3"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -478,15 +526,17 @@
     <xf numFmtId="0" fontId="12" fillId="7" borderId="9" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="6" xfId="6"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Accent1" xfId="5" builtinId="29"/>
+    <cellStyle name="Check Cell" xfId="6" builtinId="23"/>
     <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -695,6 +745,976 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.1270874563139501E-2"/>
+          <c:y val="0.13153124999999999"/>
+          <c:w val="0.92519971367215459"/>
+          <c:h val="0.81159916338582672"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'click&amp;firefly'!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>bit reliability (%) @ 0.6m @ 24 22</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'click&amp;firefly'!$B$2:$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1k</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50k</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75k</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100k</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>125k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'click&amp;firefly'!$B$3:$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.97543352601155897</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.73271543086171897</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.4666446291399</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>61.483594864479301</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.3945739217478303</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BE4D-F344-A5D5-04756E19AD22}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'click&amp;firefly'!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>bit reliability (%) @ 0.6m @ 30 28</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'click&amp;firefly'!$B$2:$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1k</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50k</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75k</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100k</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>125k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'click&amp;firefly'!$B$4:$F$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.94521604938271298</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.98331661412056</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.39463262554768</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.63911589895988</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BE4D-F344-A5D5-04756E19AD22}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="79454991"/>
+        <c:axId val="79550191"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="79454991"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="79550191"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="79550191"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="79454991"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-SE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>311150</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92AEE5C3-3207-F5C7-DB60-317CF47C9623}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1026,7 +2046,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
@@ -1336,7 +2356,9 @@
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1369,141 +2391,156 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{411A848C-79E9-A549-AF4C-929074E1F683}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="26" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D1" s="14" t="s">
+    <row r="1" spans="1:13" ht="26" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="15" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="16"/>
       <c r="I1" s="17"/>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="18"/>
+      <c r="K1" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="L1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="12"/>
+      <c r="M1" s="8"/>
     </row>
-    <row r="2" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="7" t="s">
+    <row r="2" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="8" t="s">
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="11" t="s">
+      <c r="I2" s="13"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="11">
+      <c r="M2" s="7">
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="22" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+    <row r="3" spans="1:13" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="F3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="G3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="H3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="I3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="J3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="13"/>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="19"/>
+      <c r="L3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="11">
+      <c r="M3" s="7">
         <v>347.22222219999998</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>L6 + C4</f>
+        <f>M6 + C4</f>
         <v>2451000</v>
       </c>
       <c r="B4" cm="1">
-        <f t="array" ref="B4:B9">(H4:H9+E4:E9 )/2</f>
+        <f t="array" ref="B4:B9">(I4:I9+F4:F9 )/2</f>
         <v>0.99041445035460995</v>
       </c>
       <c r="C4">
         <v>1000</v>
       </c>
-      <c r="E4" cm="1">
-        <f t="array" ref="E4:E9">L2/F4:F9</f>
+      <c r="D4">
+        <v>0.6</v>
+      </c>
+      <c r="E4">
+        <v>0.5</v>
+      </c>
+      <c r="F4" cm="1">
+        <f t="array" ref="F4:F9">M2/G4:G9</f>
         <v>0.65104166666666663</v>
       </c>
-      <c r="F4" cm="1">
-        <f t="array" ref="F4:F9">EVEN((1000 * L2)/(C4:C9 - L3))</f>
+      <c r="G4" cm="1">
+        <f t="array" ref="G4:G9">EVEN((1000 * M2)/(C4:C9 - M3))</f>
         <v>192</v>
       </c>
-      <c r="H4" cm="1">
-        <f t="array" ref="H4:H9" xml:space="preserve"> L2/I4:I9</f>
+      <c r="H4" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="I4" cm="1">
+        <f t="array" ref="I4:I9" xml:space="preserve"> M2/J4:J9</f>
         <v>1.3297872340425532</v>
       </c>
-      <c r="I4" cm="1">
-        <f t="array" ref="I4:I9">EVEN((1000 * L2)/(C4:C9 + L3))</f>
+      <c r="J4" cm="1">
+        <f t="array" ref="J4:J9">EVEN((1000 * M2)/(C4:C9 + M3))</f>
         <v>94</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="L4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="11">
-        <f>2 *L3 + L5</f>
+      <c r="M4" s="7">
+        <f>2 *M3 + M5</f>
         <v>794.44444439999995</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>L6 + C5</f>
+        <f>M6 + C5</f>
         <v>2452000</v>
       </c>
       <c r="B5">
@@ -1512,28 +2549,31 @@
       <c r="C5">
         <v>2000</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>1.6447368421052631</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>76</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="I5">
         <v>2.3148148148148149</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>54</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="L5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="11">
+      <c r="M5" s="7">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f xml:space="preserve"> L6 + C6</f>
+        <f xml:space="preserve"> M6 + C6</f>
         <v>2453000</v>
       </c>
       <c r="B6">
@@ -1542,28 +2582,31 @@
       <c r="C6">
         <v>3000</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>2.6041666666666665</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>48</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="I6">
         <v>3.2894736842105261</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>38</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="L6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="11">
+      <c r="M6" s="7">
         <v>2450000</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>L6 + C7</f>
+        <f>M6 + C7</f>
         <v>2454000</v>
       </c>
       <c r="B7">
@@ -1572,22 +2615,25 @@
       <c r="C7">
         <v>4000</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>3.4722222222222223</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>36</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="I7">
         <v>4.166666666666667</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f xml:space="preserve"> L6 + C8</f>
+        <f xml:space="preserve"> M6 + C8</f>
         <v>2455000</v>
       </c>
       <c r="B8">
@@ -1596,22 +2642,25 @@
       <c r="C8">
         <v>5000</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>4.4642857142857144</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>28</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="I8">
         <v>5.208333333333333</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f>L6 + C9</f>
+        <f>M6 + C9</f>
         <v>2456000</v>
       </c>
       <c r="B9">
@@ -1620,27 +2669,120 @@
       <c r="C9">
         <v>6000</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>5.208333333333333</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>24</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="I9">
         <v>6.25</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>20</v>
       </c>
     </row>
+    <row r="10" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:J3"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C369D4D9-A069-5541-AB11-F9E0294DBD82}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>0.97543352601155897</v>
+      </c>
+      <c r="C3">
+        <v>0.73271543086171897</v>
+      </c>
+      <c r="D3">
+        <v>10.4666446291399</v>
+      </c>
+      <c r="E3">
+        <v>61.483594864479301</v>
+      </c>
+      <c r="F3">
+        <v>6.3945739217478303</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <v>0.94521604938271298</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1.98331661412056</v>
+      </c>
+      <c r="E4">
+        <v>3.39463262554768</v>
+      </c>
+      <c r="F4">
+        <v>1.63911589895988</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
conducted some experiments with 100kbps at home with clicker and firefly from a specified distance of 0.9m and 0.1m alternated the dividers from 18 up until 28
</commit_message>
<xml_diff>
--- a/stats/fieldtestingparameters.xlsx
+++ b/stats/fieldtestingparameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fadde/Projects/wcnes-project2023/stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D887A5-16FB-F549-969C-C3D53270AD33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB5B369-93E7-A645-9B95-215FA49FAE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="1840" windowWidth="31100" windowHeight="19420" activeTab="2" xr2:uid="{0E90CDDC-DED9-2445-AC68-A5DC0636EE53}"/>
+    <workbookView xWindow="17500" yWindow="3340" windowWidth="33700" windowHeight="19420" activeTab="1" xr2:uid="{0E90CDDC-DED9-2445-AC68-A5DC0636EE53}"/>
   </bookViews>
   <sheets>
     <sheet name="clicktoclick" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
   <si>
     <t>f0 divider</t>
   </si>
@@ -171,13 +171,28 @@
   </si>
   <si>
     <t>bit reliability (%) @ 0.6m @ 30 28</t>
+  </si>
+  <si>
+    <t>Firefly &amp; Clicker (fixed distance of 0.1m)</t>
+  </si>
+  <si>
+    <t>Firefly &amp; launchpad</t>
+  </si>
+  <si>
+    <t>D_0 (m)</t>
+  </si>
+  <si>
+    <t>D_1 (m)</t>
+  </si>
+  <si>
+    <t>0.9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -279,8 +294,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,8 +358,18 @@
         <fgColor rgb="FFA5A5A5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -468,8 +513,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -477,8 +551,10 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -502,6 +578,7 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="6" xfId="6"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -529,14 +606,36 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="6" xfId="6"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" xfId="7" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Accent1" xfId="5" builtinId="29"/>
+    <cellStyle name="Bad" xfId="8" builtinId="27"/>
     <cellStyle name="Check Cell" xfId="6" builtinId="23"/>
+    <cellStyle name="Good" xfId="7" builtinId="26"/>
     <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2391,309 +2490,609 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{411A848C-79E9-A549-AF4C-929074E1F683}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" style="28" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="26" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D1" s="15" t="s">
+    <row r="1" spans="1:12" ht="26" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="16" t="s">
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19" t="s">
+      <c r="H1" s="18"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="8"/>
-    </row>
-    <row r="2" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="11" t="s">
+      <c r="L1" s="8"/>
+    </row>
+    <row r="2" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12" t="s">
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="13"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="7" t="s">
+      <c r="H2" s="14"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="7">
+      <c r="L2" s="7">
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="27" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>27</v>
       </c>
       <c r="E3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="H3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="I3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="19"/>
-      <c r="L3" s="7" t="s">
+      <c r="J3" s="20"/>
+      <c r="K3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="7">
+      <c r="L3" s="7">
         <v>347.22222219999998</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>M6 + C4</f>
+        <f>L6 + C4</f>
         <v>2451000</v>
       </c>
       <c r="B4" cm="1">
-        <f t="array" ref="B4:B9">(I4:I9+F4:F9 )/2</f>
+        <f t="array" ref="B4:B9">(H4:H9+E4:E9 )/2</f>
         <v>0.99041445035460995</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="28">
         <v>1000</v>
       </c>
       <c r="D4">
         <v>0.6</v>
       </c>
-      <c r="E4">
-        <v>0.5</v>
+      <c r="E4" cm="1">
+        <f t="array" ref="E4:E9">L2/F4:F9</f>
+        <v>0.65104166666666663</v>
       </c>
       <c r="F4" cm="1">
-        <f t="array" ref="F4:F9">M2/G4:G9</f>
-        <v>0.65104166666666663</v>
-      </c>
-      <c r="G4" cm="1">
-        <f t="array" ref="G4:G9">EVEN((1000 * M2)/(C4:C9 - M3))</f>
+        <f t="array" ref="F4:F9">EVEN((1000 * L2)/(C4:C9 - L3))</f>
         <v>192</v>
       </c>
-      <c r="H4" s="20">
+      <c r="G4" s="11">
         <v>0.1</v>
       </c>
+      <c r="H4" cm="1">
+        <f t="array" ref="H4:H9" xml:space="preserve"> L2/I4:I9</f>
+        <v>1.3297872340425532</v>
+      </c>
       <c r="I4" cm="1">
-        <f t="array" ref="I4:I9" xml:space="preserve"> M2/J4:J9</f>
-        <v>1.3297872340425532</v>
-      </c>
-      <c r="J4" cm="1">
-        <f t="array" ref="J4:J9">EVEN((1000 * M2)/(C4:C9 + M3))</f>
+        <f t="array" ref="I4:I9">EVEN((1000 * L2)/(C4:C9 + L3))</f>
         <v>94</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="K4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="7">
-        <f>2 *M3 + M5</f>
+      <c r="L4" s="7">
+        <f>2 *L3 + L5</f>
         <v>794.44444439999995</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>M6 + C5</f>
+        <f>L6 + C5</f>
         <v>2452000</v>
       </c>
       <c r="B5">
         <v>1.9797758284600389</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="28">
         <v>2000</v>
       </c>
+      <c r="E5">
+        <v>1.6447368421052631</v>
+      </c>
       <c r="F5">
-        <v>1.6447368421052631</v>
-      </c>
-      <c r="G5">
         <v>76</v>
       </c>
-      <c r="H5" s="20">
+      <c r="G5" s="11">
         <v>0.1</v>
       </c>
+      <c r="H5">
+        <v>2.3148148148148149</v>
+      </c>
       <c r="I5">
-        <v>2.3148148148148149</v>
-      </c>
-      <c r="J5">
         <v>54</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="K5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="7">
+      <c r="L5" s="7">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f xml:space="preserve"> M6 + C6</f>
+        <f xml:space="preserve"> L6 + C6</f>
         <v>2453000</v>
       </c>
       <c r="B6">
         <v>2.9468201754385963</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="28">
         <v>3000</v>
       </c>
+      <c r="E6">
+        <v>2.6041666666666665</v>
+      </c>
       <c r="F6">
-        <v>2.6041666666666665</v>
-      </c>
-      <c r="G6">
         <v>48</v>
       </c>
-      <c r="H6" s="20">
+      <c r="G6" s="11">
         <v>0.1</v>
       </c>
+      <c r="H6">
+        <v>3.2894736842105261</v>
+      </c>
       <c r="I6">
-        <v>3.2894736842105261</v>
-      </c>
-      <c r="J6">
         <v>38</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="K6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="7">
+      <c r="L6" s="7">
         <v>2450000</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>M6 + C7</f>
+        <f>L6 + C7</f>
         <v>2454000</v>
       </c>
       <c r="B7">
         <v>3.8194444444444446</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="28">
         <v>4000</v>
       </c>
+      <c r="E7">
+        <v>3.4722222222222223</v>
+      </c>
       <c r="F7">
-        <v>3.4722222222222223</v>
-      </c>
-      <c r="G7">
         <v>36</v>
       </c>
-      <c r="H7" s="20">
+      <c r="G7" s="11">
         <v>0.1</v>
       </c>
+      <c r="H7">
+        <v>4.166666666666667</v>
+      </c>
       <c r="I7">
-        <v>4.166666666666667</v>
-      </c>
-      <c r="J7">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f xml:space="preserve"> M6 + C8</f>
+        <f xml:space="preserve"> L6 + C8</f>
         <v>2455000</v>
       </c>
       <c r="B8">
         <v>4.8363095238095237</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="28">
         <v>5000</v>
       </c>
+      <c r="E8">
+        <v>4.4642857142857144</v>
+      </c>
       <c r="F8">
-        <v>4.4642857142857144</v>
-      </c>
-      <c r="G8">
         <v>28</v>
       </c>
-      <c r="H8" s="20">
+      <c r="G8" s="11">
         <v>0.1</v>
       </c>
+      <c r="H8">
+        <v>5.208333333333333</v>
+      </c>
       <c r="I8">
-        <v>5.208333333333333</v>
-      </c>
-      <c r="J8">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f>M6 + C9</f>
+        <f>L6 + C9</f>
         <v>2456000</v>
       </c>
       <c r="B9">
         <v>5.7291666666666661</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="28">
         <v>6000</v>
       </c>
+      <c r="E9">
+        <v>5.208333333333333</v>
+      </c>
       <c r="F9">
+        <v>24</v>
+      </c>
+      <c r="G9" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="H9">
+        <v>6.25</v>
+      </c>
+      <c r="I9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
+    </row>
+    <row r="16" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
+    </row>
+    <row r="17" spans="1:12" ht="26" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="22"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="18"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="L17" s="8"/>
+    </row>
+    <row r="18" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="25"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="14"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L18" s="7">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" s="20"/>
+      <c r="K19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L19" s="7">
+        <v>347.22222219999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="29">
+        <f>L22 + C20</f>
+        <v>2451000</v>
+      </c>
+      <c r="B20" s="29" cm="1">
+        <f t="array" ref="B20:B25">(H20:H25+E20:E25 )/2</f>
+        <v>4.6359890109890109</v>
+      </c>
+      <c r="C20" s="29">
+        <v>1000</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="29" cm="1">
+        <f t="array" ref="E20:E25">L18/F20:F25</f>
+        <v>4.4642857142857144</v>
+      </c>
+      <c r="F20" s="29">
+        <v>28</v>
+      </c>
+      <c r="G20" s="30">
+        <v>0.1</v>
+      </c>
+      <c r="H20" s="29" cm="1">
+        <f t="array" ref="H20:H25" xml:space="preserve"> L18/I20:I25</f>
+        <v>4.8076923076923075</v>
+      </c>
+      <c r="I20" s="29">
+        <v>26</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L20" s="7">
+        <f>2 *L19 + L21</f>
+        <v>794.44444439999995</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f>L22 + C21</f>
+        <v>2452000</v>
+      </c>
+      <c r="B21">
+        <v>5.0080128205128203</v>
+      </c>
+      <c r="C21" s="28">
+        <v>2000</v>
+      </c>
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21">
+        <v>4.8076923076923075</v>
+      </c>
+      <c r="F21">
+        <v>26</v>
+      </c>
+      <c r="G21" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="H21">
         <v>5.208333333333333</v>
       </c>
-      <c r="G9">
+      <c r="I21">
         <v>24</v>
       </c>
-      <c r="H9" s="20">
+      <c r="K21" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L21" s="7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f xml:space="preserve"> L22 + C22</f>
+        <v>2453000</v>
+      </c>
+      <c r="B22">
+        <v>5.4450757575757578</v>
+      </c>
+      <c r="C22" s="28">
+        <v>3000</v>
+      </c>
+      <c r="D22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22">
+        <v>5.208333333333333</v>
+      </c>
+      <c r="F22">
+        <v>24</v>
+      </c>
+      <c r="G22" s="11">
         <v>0.1</v>
       </c>
-      <c r="I9">
+      <c r="H22">
+        <v>5.6818181818181817</v>
+      </c>
+      <c r="I22">
+        <v>22</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L22" s="7">
+        <v>2450000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f>L22 + C23</f>
+        <v>2454000</v>
+      </c>
+      <c r="B23">
+        <v>5.9659090909090908</v>
+      </c>
+      <c r="C23" s="28">
+        <v>4000</v>
+      </c>
+      <c r="D23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23">
+        <v>5.6818181818181817</v>
+      </c>
+      <c r="F23">
+        <v>22</v>
+      </c>
+      <c r="G23" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="H23">
         <v>6.25</v>
       </c>
-      <c r="J9">
+      <c r="I23">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f xml:space="preserve"> L22 + C24</f>
+        <v>2455000</v>
+      </c>
+      <c r="B24">
+        <v>6.5972222222222223</v>
+      </c>
+      <c r="C24" s="28">
+        <v>5000</v>
+      </c>
+      <c r="D24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24">
+        <v>6.25</v>
+      </c>
+      <c r="F24">
+        <v>20</v>
+      </c>
+      <c r="G24" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="H24">
+        <v>6.9444444444444446</v>
+      </c>
+      <c r="I24">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f>L22 + C25</f>
+        <v>2456000</v>
+      </c>
+      <c r="B25">
+        <v>7.3784722222222223</v>
+      </c>
+      <c r="C25" s="28">
+        <v>6000</v>
+      </c>
+      <c r="D25" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25">
+        <v>6.9444444444444446</v>
+      </c>
+      <c r="F25">
+        <v>18</v>
+      </c>
+      <c r="G25" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="H25">
+        <v>7.8125</v>
+      </c>
+      <c r="I25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:K3"/>
+  <mergeCells count="12">
+    <mergeCell ref="A17:C18"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="J17:J19"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:J3"/>
   </mergeCells>
+  <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2702,8 +3101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C369D4D9-A069-5541-AB11-F9E0294DBD82}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>